<commit_message>
The code was edited to make it easier to modify and a new model was additionally learned.
</commit_message>
<xml_diff>
--- a/Model information/Performance by model.xlsx
+++ b/Model information/Performance by model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\Model Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF150A2-F571-4364-AE43-25C23689D24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726E123D-70BC-4ACB-9DCC-199CDA2F7E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="2010" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="4530" yWindow="1080" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -592,10 +592,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="2">
-        <v>0.73309999999999997</v>
+        <v>0.64459999999999995</v>
       </c>
       <c r="F2" s="2">
-        <v>0.75580000000000003</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -612,10 +612,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="2">
-        <v>0.55579999999999996</v>
+        <v>0.49959999999999999</v>
       </c>
       <c r="F3" s="2">
-        <v>0.8135</v>
+        <v>0.81730000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -631,12 +631,8 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.55730000000000002</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.7923</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -651,12 +647,8 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.51370000000000005</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.83079999999999998</v>
-      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -671,12 +663,8 @@
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
-        <v>1.4461999999999999</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.39040000000000002</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -691,12 +679,8 @@
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.54590000000000005</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.79420000000000002</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -711,12 +695,8 @@
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.56930000000000003</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.79810000000000003</v>
-      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -732,10 +712,10 @@
         <v>25</v>
       </c>
       <c r="E9" s="2">
-        <v>0.54800000000000004</v>
+        <v>0.44379999999999997</v>
       </c>
       <c r="F9" s="2">
-        <v>0.80579999999999996</v>
+        <v>0.83079999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -751,12 +731,8 @@
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.47260000000000002</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.84419999999999995</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -771,12 +747,8 @@
       <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2">
-        <v>1.6758999999999999</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.26150000000000001</v>
-      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
A new model was additionally trained.
</commit_message>
<xml_diff>
--- a/Model information/Performance by model.xlsx
+++ b/Model information/Performance by model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\Model Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726E123D-70BC-4ACB-9DCC-199CDA2F7E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94FE1EC-335D-40B0-B784-B86AC55F1402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="1080" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -631,8 +631,12 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2">
+        <v>0.45140000000000002</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.84619999999999995</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -647,8 +651,12 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.82789999999999997</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">

</xml_diff>